<commit_message>
Updatred envt to sandbox
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation\NewArrivals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\testautomation\KatalonProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>firstName</t>
   </si>
@@ -109,6 +109,30 @@
   </si>
   <si>
     <t>Florida</t>
+  </si>
+  <si>
+    <t>sushanthost</t>
+  </si>
+  <si>
+    <t>sushantguest1</t>
+  </si>
+  <si>
+    <t>sushantguest2</t>
+  </si>
+  <si>
+    <t>sushanthost@test.com</t>
+  </si>
+  <si>
+    <t>sushantguest1@test.com</t>
+  </si>
+  <si>
+    <t>sushantguest2@test.com</t>
+  </si>
+  <si>
+    <t>sushantcohost</t>
+  </si>
+  <si>
+    <t>sushantcohost@test.com</t>
   </si>
 </sst>
 </file>
@@ -559,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D10" sqref="D10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -712,6 +736,98 @@
         <v>48085</v>
       </c>
     </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7">
+        <v>48085</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8">
+        <v>48085</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>48085</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>48085</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
@@ -720,9 +836,12 @@
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Major updates in NA scripts
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>firstName</t>
   </si>
@@ -45,46 +45,40 @@
     <t>abc</t>
   </si>
   <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>TROY</t>
-  </si>
-  <si>
-    <t>cohost-test</t>
-  </si>
-  <si>
-    <t>guest1-test</t>
-  </si>
-  <si>
-    <t>guest2-test</t>
-  </si>
-  <si>
-    <t>973 BRAHMS CT</t>
-  </si>
-  <si>
-    <t>974 BRAHMS CT</t>
-  </si>
-  <si>
-    <t>975 BRAHMS CT</t>
-  </si>
-  <si>
-    <t>976 BRAHMS CT</t>
-  </si>
-  <si>
-    <t>hostess-test</t>
-  </si>
-  <si>
-    <t>hostess-test@test.com</t>
-  </si>
-  <si>
-    <t>cohost-test@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test@test.com</t>
-  </si>
-  <si>
-    <t>guest2-test@test.com</t>
+    <t>450 KIPLING AVE</t>
+  </si>
+  <si>
+    <t>ETOBICOKE</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>M8Z 5E1</t>
+  </si>
+  <si>
+    <t>ahostess-test1</t>
+  </si>
+  <si>
+    <t>ahostess-test1@test.com</t>
+  </si>
+  <si>
+    <t>bcohost-test1</t>
+  </si>
+  <si>
+    <t>bcohost-test1@test.com</t>
+  </si>
+  <si>
+    <t>guest1-test1</t>
+  </si>
+  <si>
+    <t>guest1-test1@test.com</t>
+  </si>
+  <si>
+    <t>guest2-test1</t>
+  </si>
+  <si>
+    <t>guest2-test1@test.com</t>
   </si>
 </sst>
 </file>
@@ -159,11 +153,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -535,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -574,160 +567,96 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>48085</v>
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3">
-        <v>48085</v>
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4">
-        <v>48085</v>
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5">
-        <v>48085</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
updated NA US scripts
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>firstName</t>
   </si>
@@ -45,37 +45,43 @@
     <t>abc</t>
   </si>
   <si>
-    <t>450 KIPLING AVE</t>
-  </si>
-  <si>
-    <t>ETOBICOKE</t>
-  </si>
-  <si>
-    <t>Ontario</t>
-  </si>
-  <si>
-    <t>M8Z 5E1</t>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>TROY</t>
+  </si>
+  <si>
+    <t>973 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>974 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>975 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>976 BRAHMS CT</t>
   </si>
   <si>
     <t>ahostess-test1</t>
   </si>
   <si>
+    <t>bcohost-test1</t>
+  </si>
+  <si>
+    <t>guest1-test1</t>
+  </si>
+  <si>
+    <t>guest2-test1</t>
+  </si>
+  <si>
     <t>ahostess-test1@test.com</t>
   </si>
   <si>
-    <t>bcohost-test1</t>
-  </si>
-  <si>
     <t>bcohost-test1@test.com</t>
   </si>
   <si>
-    <t>guest1-test1</t>
-  </si>
-  <si>
     <t>guest1-test1@test.com</t>
-  </si>
-  <si>
-    <t>guest2-test1</t>
   </si>
   <si>
     <t>guest2-test1@test.com</t>
@@ -531,7 +537,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -568,48 +574,48 @@
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>48085</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>48085</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -620,42 +626,42 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>48085</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>48085</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated NA scripts: addOn scripts
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>firstName</t>
   </si>
@@ -45,53 +45,47 @@
     <t>abc</t>
   </si>
   <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>TROY</t>
-  </si>
-  <si>
-    <t>973 BRAHMS CT</t>
-  </si>
-  <si>
-    <t>974 BRAHMS CT</t>
-  </si>
-  <si>
-    <t>975 BRAHMS CT</t>
-  </si>
-  <si>
-    <t>976 BRAHMS CT</t>
-  </si>
-  <si>
-    <t>ahostess-test</t>
+    <t>80 Rowton</t>
+  </si>
+  <si>
+    <t>Chester</t>
+  </si>
+  <si>
+    <t>CH3 0FS</t>
+  </si>
+  <si>
+    <t>GB-CHES</t>
   </si>
   <si>
     <t>bcohost-test</t>
   </si>
   <si>
+    <t>bcohost-test@test.com</t>
+  </si>
+  <si>
     <t>guest1-test</t>
   </si>
   <si>
+    <t>guest1-test@test.com</t>
+  </si>
+  <si>
     <t>guest2-test</t>
   </si>
   <si>
-    <t>ahostess-test@test.com</t>
-  </si>
-  <si>
-    <t>bcohost-test@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test@test.com</t>
-  </si>
-  <si>
     <t>guest2-test@test.com</t>
+  </si>
+  <si>
+    <t>ahostess-test1</t>
+  </si>
+  <si>
+    <t>ahostess-test1@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -107,6 +101,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -159,7 +159,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
@@ -167,6 +167,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -537,7 +538,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D14:D15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -572,96 +573,96 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>48085</v>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3">
-        <v>48085</v>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4">
-        <v>48085</v>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5">
-        <v>48085</v>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
userRegistraion updated: using JavaScript
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>firstName</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>guest3-test@test.com</t>
+  </si>
+  <si>
+    <t>blackdress19</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -540,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -553,9 +559,11 @@
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="36.140625" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,8 +585,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -600,8 +611,11 @@
       <c r="G2">
         <v>48085</v>
       </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -623,8 +637,11 @@
       <c r="G3">
         <v>48085</v>
       </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -646,8 +663,11 @@
       <c r="G4">
         <v>48085</v>
       </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -669,8 +689,11 @@
       <c r="G5">
         <v>48085</v>
       </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
@@ -691,6 +714,9 @@
       </c>
       <c r="G6">
         <v>48085</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
productVerify and BORetail updated: stale element exception handled
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -63,40 +63,40 @@
     <t>976 BRAHMS CT</t>
   </si>
   <si>
-    <t>ahostess-test</t>
-  </si>
-  <si>
-    <t>bcohost-test</t>
-  </si>
-  <si>
-    <t>guest1-test</t>
-  </si>
-  <si>
-    <t>guest2-test</t>
-  </si>
-  <si>
-    <t>ahostess-test@test.com</t>
-  </si>
-  <si>
-    <t>bcohost-test@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test@test.com</t>
-  </si>
-  <si>
-    <t>guest2-test@test.com</t>
-  </si>
-  <si>
-    <t>guest3-test</t>
-  </si>
-  <si>
-    <t>guest3-test@test.com</t>
-  </si>
-  <si>
     <t>blackdress19</t>
   </si>
   <si>
     <t>pass</t>
+  </si>
+  <si>
+    <t>ahostess-test1</t>
+  </si>
+  <si>
+    <t>ahostess-test1@test.com</t>
+  </si>
+  <si>
+    <t>bcohost-test1@test.com</t>
+  </si>
+  <si>
+    <t>guest1-test1@test.com</t>
+  </si>
+  <si>
+    <t>guest2-test1@test.com</t>
+  </si>
+  <si>
+    <t>guest3-test1@test.com</t>
+  </si>
+  <si>
+    <t>bcohost-test1</t>
+  </si>
+  <si>
+    <t>guest1-test1</t>
+  </si>
+  <si>
+    <t>guest2-test1</t>
+  </si>
+  <si>
+    <t>guest3-test1</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -586,18 +586,18 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -612,18 +612,18 @@
         <v>48085</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -638,18 +638,18 @@
         <v>48085</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
@@ -664,18 +664,18 @@
         <v>48085</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>13</v>
@@ -690,18 +690,18 @@
         <v>48085</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>13</v>
@@ -716,7 +716,7 @@
         <v>48085</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
urgent stress test suite collection
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>firstName</t>
   </si>
@@ -45,40 +45,55 @@
     <t>abc</t>
   </si>
   <si>
-    <t>450 KIPLING AVE</t>
-  </si>
-  <si>
-    <t>ETOBICOKE</t>
-  </si>
-  <si>
-    <t>Ontario</t>
-  </si>
-  <si>
-    <t>M8Z 5E1</t>
-  </si>
-  <si>
-    <t>ahostess-test2</t>
-  </si>
-  <si>
-    <t>ahostess-test3@test.com</t>
-  </si>
-  <si>
-    <t>bcohost-test3@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test3@test.com</t>
-  </si>
-  <si>
-    <t>guest2-test3@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test1</t>
-  </si>
-  <si>
-    <t>bcohost-test1</t>
-  </si>
-  <si>
-    <t>guest2-test1</t>
+    <t>973 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>TROY</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>blackdress19</t>
+  </si>
+  <si>
+    <t>974 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>975 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>976 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>ahostess-test</t>
+  </si>
+  <si>
+    <t>ahostess-test@test.com</t>
+  </si>
+  <si>
+    <t>bcohost-test</t>
+  </si>
+  <si>
+    <t>bcohost-test@test.com</t>
+  </si>
+  <si>
+    <t>guest1-test</t>
+  </si>
+  <si>
+    <t>guest1-test@test.com</t>
+  </si>
+  <si>
+    <t>guest2-test</t>
+  </si>
+  <si>
+    <t>guest2-test@test.com</t>
+  </si>
+  <si>
+    <t>guest3-test</t>
+  </si>
+  <si>
+    <t>guest3-test@test.com</t>
   </si>
 </sst>
 </file>
@@ -528,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -543,7 +558,7 @@
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,15 +581,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -585,22 +600,25 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>48085</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -608,22 +626,25 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>48085</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -631,22 +652,25 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>48085</v>
+      </c>
+      <c r="H4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -654,20 +678,50 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>48085</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>48085</v>
+      </c>
+      <c r="H6" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" display="ahostess-test3@test.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="bcohost-test3@test.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="guest1-test3@test.com"/>
+    <hyperlink ref="C5" r:id="rId4" display="guest2-test3@test.com"/>
+    <hyperlink ref="C6" r:id="rId5" display="guest3-test1@test.com"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
userRegistraion (through mail) completed
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>firstName</t>
   </si>
@@ -45,40 +45,58 @@
     <t>abc</t>
   </si>
   <si>
-    <t>450 KIPLING AVE</t>
-  </si>
-  <si>
-    <t>ETOBICOKE</t>
-  </si>
-  <si>
-    <t>Ontario</t>
-  </si>
-  <si>
-    <t>M8Z 5E1</t>
-  </si>
-  <si>
-    <t>ahostess-test3@test.com</t>
-  </si>
-  <si>
-    <t>bcohost-test3@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test3@test.com</t>
-  </si>
-  <si>
-    <t>guest2-test3@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test1</t>
-  </si>
-  <si>
-    <t>bcohost-test1</t>
-  </si>
-  <si>
-    <t>guest2-test1</t>
-  </si>
-  <si>
-    <t>ahostess-test1</t>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>ahostess-test</t>
+  </si>
+  <si>
+    <t>ahostess-test@test.com</t>
+  </si>
+  <si>
+    <t>973 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>TROY</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>blackdress19</t>
+  </si>
+  <si>
+    <t>bcohost-test</t>
+  </si>
+  <si>
+    <t>bcohost-test@test.com</t>
+  </si>
+  <si>
+    <t>974 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>guest1-test</t>
+  </si>
+  <si>
+    <t>guest1-test@test.com</t>
+  </si>
+  <si>
+    <t>975 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>guest2-test</t>
+  </si>
+  <si>
+    <t>guest2-test@test.com</t>
+  </si>
+  <si>
+    <t>976 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>guest3-test</t>
+  </si>
+  <si>
+    <t>guest3-test@test.com</t>
   </si>
 </sst>
 </file>
@@ -528,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -541,9 +559,11 @@
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="36.140625" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,97 +585,138 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>48085</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
+      <c r="G3">
+        <v>48085</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>48085</v>
+      </c>
+      <c r="H4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>48085</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>48085</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -665,9 +726,10 @@
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
VS_Automation updated: webui.click is changed to java executor click method
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>firstName</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>guest3-test@test.com</t>
+  </si>
+  <si>
+    <t>974 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>975 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>976 BRAHMS CT</t>
   </si>
 </sst>
 </file>
@@ -633,7 +642,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -659,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -685,7 +694,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
product verify updated to handle 'stale element exception' (some element actions are updated to consider newly created TO)
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -48,12 +48,6 @@
     <t>pass</t>
   </si>
   <si>
-    <t>ahostess-test</t>
-  </si>
-  <si>
-    <t>ahostess-test@test.com</t>
-  </si>
-  <si>
     <t>973 BRAHMS CT</t>
   </si>
   <si>
@@ -66,30 +60,6 @@
     <t>blackdress19</t>
   </si>
   <si>
-    <t>bcohost-test</t>
-  </si>
-  <si>
-    <t>bcohost-test@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test</t>
-  </si>
-  <si>
-    <t>guest1-test@test.com</t>
-  </si>
-  <si>
-    <t>guest2-test</t>
-  </si>
-  <si>
-    <t>guest2-test@test.com</t>
-  </si>
-  <si>
-    <t>guest3-test</t>
-  </si>
-  <si>
-    <t>guest3-test@test.com</t>
-  </si>
-  <si>
     <t>974 BRAHMS CT</t>
   </si>
   <si>
@@ -97,6 +67,36 @@
   </si>
   <si>
     <t>976 BRAHMS CT</t>
+  </si>
+  <si>
+    <t>ahostess-test1</t>
+  </si>
+  <si>
+    <t>bcohost-test1</t>
+  </si>
+  <si>
+    <t>guest1-test1</t>
+  </si>
+  <si>
+    <t>guest2-test1</t>
+  </si>
+  <si>
+    <t>guest3-test1</t>
+  </si>
+  <si>
+    <t>ahostess-test1@test.com</t>
+  </si>
+  <si>
+    <t>bcohost-test1@test.com</t>
+  </si>
+  <si>
+    <t>guest1-test1@test.com</t>
+  </si>
+  <si>
+    <t>guest2-test1@test.com</t>
+  </si>
+  <si>
+    <t>guest3-test1@test.com</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -581,80 +581,80 @@
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
       </c>
       <c r="G2">
         <v>48085</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
       </c>
       <c r="G3">
         <v>48085</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>48085</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -665,48 +665,48 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>48085</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>48085</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Contact suite created
</commit_message>
<xml_diff>
--- a/KatalonProjects/contactData.xlsx
+++ b/KatalonProjects/contactData.xlsx
@@ -69,41 +69,41 @@
     <t>976 BRAHMS CT</t>
   </si>
   <si>
-    <t>ahostess-test1</t>
-  </si>
-  <si>
-    <t>bcohost-test1</t>
-  </si>
-  <si>
-    <t>guest1-test1</t>
-  </si>
-  <si>
-    <t>guest2-test1</t>
-  </si>
-  <si>
-    <t>guest3-test1</t>
-  </si>
-  <si>
-    <t>ahostess-test1@test.com</t>
-  </si>
-  <si>
-    <t>bcohost-test1@test.com</t>
-  </si>
-  <si>
-    <t>guest1-test1@test.com</t>
-  </si>
-  <si>
-    <t>guest2-test1@test.com</t>
-  </si>
-  <si>
-    <t>guest3-test1@test.com</t>
+    <t>ahostess-test</t>
+  </si>
+  <si>
+    <t>bcohost-test</t>
+  </si>
+  <si>
+    <t>guest1-test</t>
+  </si>
+  <si>
+    <t>guest2-test</t>
+  </si>
+  <si>
+    <t>guest3-test</t>
+  </si>
+  <si>
+    <t>ahostess-test@test.com</t>
+  </si>
+  <si>
+    <t>bcohost-test@test.com</t>
+  </si>
+  <si>
+    <t>guest1-test@test.com</t>
+  </si>
+  <si>
+    <t>guest2-test@test.com</t>
+  </si>
+  <si>
+    <t>guest3-test@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -113,6 +113,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -159,20 +166,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -539,7 +549,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -586,7 +596,7 @@
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -612,7 +622,7 @@
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -638,7 +648,7 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -664,7 +674,7 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -690,7 +700,7 @@
       <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -711,8 +721,15 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>